<commit_message>
Atualização das cotações por meio de macro em outra planilha
</commit_message>
<xml_diff>
--- a/ArquivoExcel/Cotações.xlsx
+++ b/ArquivoExcel/Cotações.xlsx
@@ -461,10 +461,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.04354</v>
+        <v>5.8576</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45756.50506039</v>
+        <v>45759.91172538449</v>
       </c>
     </row>
     <row r="3">
@@ -474,10 +474,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.67557</v>
+        <v>6.65779</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45756.50506039</v>
+        <v>45759.91172538449</v>
       </c>
     </row>
     <row r="4">
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>468756000</v>
+        <v>502853000</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45756.50506039</v>
+        <v>45759.91172538449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização nome botão macro e atualização de valores monetários
</commit_message>
<xml_diff>
--- a/ArquivoExcel/Cotações.xlsx
+++ b/ArquivoExcel/Cotações.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
         <v>5.8576</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45759.91172538449</v>
+        <v>45759.91172538194</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         <v>6.65779</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45759.91172538449</v>
+        <v>45759.91172538194</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,46 @@
         <v>502853000</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45759.91172538449</v>
+        <v>45759.91172538194</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dólar</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5.8546</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45761.82636843352</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>6.64011</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45761.82636843352</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bitcoin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>497501000</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45761.82636843352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>